<commit_message>
FInal Commit for Project.
All done for the given project. Rest easy. May comeback to fix up some things.
</commit_message>
<xml_diff>
--- a/outputs/mean_variance.xlsx
+++ b/outputs/mean_variance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{A007C239-057E-4D30-A33C-E2002EEBAA48}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FInal Sheet" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>poisson Disc samples accuracy</t>
   </si>
@@ -48,6 +49,30 @@
   </si>
   <si>
     <t>std div</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>StDev</t>
+  </si>
+  <si>
+    <t>Pure GS</t>
+  </si>
+  <si>
+    <t>PD H Reg.</t>
+  </si>
+  <si>
+    <t>GS H Reg.</t>
+  </si>
+  <si>
+    <t>PD H Log.</t>
+  </si>
+  <si>
+    <t>GS H Log.</t>
+  </si>
+  <si>
+    <t>Pure PD</t>
   </si>
 </sst>
 </file>
@@ -398,10 +423,486 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF86CC20-5345-4DE5-963C-483EAF160862}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="8.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C2">
+        <v>35.5</v>
+      </c>
+      <c r="D2">
+        <v>36.1</v>
+      </c>
+      <c r="E2">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C3">
+        <v>34.6</v>
+      </c>
+      <c r="D3">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E3">
+        <v>35.9</v>
+      </c>
+      <c r="F3">
+        <v>35.6</v>
+      </c>
+      <c r="G3">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>33.5</v>
+      </c>
+      <c r="C4">
+        <v>36.4</v>
+      </c>
+      <c r="D4">
+        <v>35.4</v>
+      </c>
+      <c r="E4">
+        <v>36.6</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>33.6</v>
+      </c>
+      <c r="C5">
+        <v>35</v>
+      </c>
+      <c r="D5">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="E5">
+        <v>35.4</v>
+      </c>
+      <c r="F5">
+        <v>35.4</v>
+      </c>
+      <c r="G5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>34.5</v>
+      </c>
+      <c r="C6">
+        <v>36.9</v>
+      </c>
+      <c r="D6">
+        <v>36.9</v>
+      </c>
+      <c r="E6">
+        <v>35.4</v>
+      </c>
+      <c r="F6">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G6">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>34.6</v>
+      </c>
+      <c r="C7">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="D7">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E7">
+        <v>35.4</v>
+      </c>
+      <c r="F7">
+        <v>36.6</v>
+      </c>
+      <c r="G7">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>34.9</v>
+      </c>
+      <c r="C8">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="D8">
+        <v>35.9</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>37.6</v>
+      </c>
+      <c r="G8">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>34.4</v>
+      </c>
+      <c r="C9">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="D9">
+        <v>34.4</v>
+      </c>
+      <c r="E9">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F9">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G9">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>34.9</v>
+      </c>
+      <c r="C10">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="D10">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="E10">
+        <v>36</v>
+      </c>
+      <c r="F10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>34.6</v>
+      </c>
+      <c r="C11">
+        <v>36.1</v>
+      </c>
+      <c r="D11">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E11">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="F11">
+        <v>36.6</v>
+      </c>
+      <c r="G11">
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="C12">
+        <v>37.5</v>
+      </c>
+      <c r="D12">
+        <v>36.1</v>
+      </c>
+      <c r="E12">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F12">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G12">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="C13">
+        <v>35.9</v>
+      </c>
+      <c r="D13">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F13">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="G13">
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>37.1</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+      <c r="D14">
+        <v>36.4</v>
+      </c>
+      <c r="E14">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="F14">
+        <v>37.5</v>
+      </c>
+      <c r="G14">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <v>35.9</v>
+      </c>
+      <c r="D15">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E15">
+        <v>35.6</v>
+      </c>
+      <c r="F15">
+        <v>33.6</v>
+      </c>
+      <c r="G15">
+        <v>32.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>33.9</v>
+      </c>
+      <c r="C16">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="D16">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="E16">
+        <v>36.1</v>
+      </c>
+      <c r="F16">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="G16">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(B2:B16)</f>
+        <v>34.76</v>
+      </c>
+      <c r="C17">
+        <f>AVERAGE(C2:C16)</f>
+        <v>36.006666666666661</v>
+      </c>
+      <c r="D17">
+        <f>AVERAGE(D2:D16)</f>
+        <v>35.506666666666668</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(E2:E16)</f>
+        <v>35.733333333333334</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F2:F16)</f>
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G17">
+        <f>AVERAGE(G2:G16)</f>
+        <v>33.453333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <f>_xlfn.VAR.S(B2:B16)</f>
+        <v>0.80542857142857149</v>
+      </c>
+      <c r="C18">
+        <f>_xlfn.VAR.S(C2:C16)</f>
+        <v>0.71495238095238123</v>
+      </c>
+      <c r="D18">
+        <f>_xlfn.VAR.S(D2:D16)</f>
+        <v>0.7492380952380947</v>
+      </c>
+      <c r="E18">
+        <f>_xlfn.VAR.S(E2:E16)</f>
+        <v>0.24238095238095256</v>
+      </c>
+      <c r="F18">
+        <f>_xlfn.VAR.S(F2:F16)</f>
+        <v>1.3142857142857152</v>
+      </c>
+      <c r="G18">
+        <f>_xlfn.VAR.S(G2:G16)</f>
+        <v>1.36552380952381</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>_xlfn.STDEV.S(B2:B16)</f>
+        <v>0.89745672398649479</v>
+      </c>
+      <c r="C19">
+        <f>_xlfn.STDEV.S(C2:C16)</f>
+        <v>0.84554856806240364</v>
+      </c>
+      <c r="D19">
+        <f>_xlfn.STDEV.S(D2:D16)</f>
+        <v>0.8655854060912157</v>
+      </c>
+      <c r="E19">
+        <f>_xlfn.STDEV.S(E2:E16)</f>
+        <v>0.49232200070782189</v>
+      </c>
+      <c r="F19">
+        <f>_xlfn.STDEV.S(F2:F16)</f>
+        <v>1.146423008442222</v>
+      </c>
+      <c r="G19">
+        <f>_xlfn.STDEV.S(G2:G16)</f>
+        <v>1.1685562928347997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEAF39B-6C10-4502-B2CC-1027B9E1C9EB}">
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E144"/>
     </sheetView>
   </sheetViews>

</xml_diff>